<commit_message>
Consolidated Transmitter Board BOM with master BOM
</commit_message>
<xml_diff>
--- a/ACDC/Project Outputs for ACDC/ACDC.xlsx
+++ b/ACDC/Project Outputs for ACDC/ACDC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr3de\Documents\MASA\2020-21-PCBs\ACDC\Project Outputs for ACDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C3CD40B-3E2C-4FCA-A9AD-0AC1258A984A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{17D81DEC-9BB3-4ACB-A4FB-63C7F14EA9E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{D24AC2E5-4D69-4F47-9D68-7C6EF3866D9C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -75,16 +75,16 @@
     <t>HX1188FNL</t>
   </si>
   <si>
+    <t>D5V0L2B3W-7</t>
+  </si>
+  <si>
     <t>M20048-1</t>
   </si>
   <si>
-    <t>SN74LVC1T45DBVR</t>
-  </si>
-  <si>
-    <t>D5V0L2B3W-7</t>
-  </si>
-  <si>
-    <t>SN65HVD1050D</t>
+    <t>MCP2515-I/SO</t>
+  </si>
+  <si>
+    <t>TCAN334DR</t>
   </si>
   <si>
     <t>TMP235A2DBZR</t>
@@ -120,10 +120,7 @@
     <t>Telecom Transformer 1:1/1:1, -40 to 85 degC, 16-Pin SMT, RoHS, Tube</t>
   </si>
   <si>
-    <t>Single-Bit Dual-Supply Bus Transceiver with Configurable Voltage Translation and 3-State Outputs, DBV0006A, LARGE T&amp;R</t>
-  </si>
-  <si>
-    <t>High-Speed EMC Optimized CAN Transceiver, 70 mA, 5 V, -40 to 125 degC, 8-pin SOIC (D), Green (RoHS &amp; no Sb/Br)</t>
+    <t>Stand-Alone CAN Controller With SPI Interface, 18-Pin SOIC, Industrial Temperature</t>
   </si>
   <si>
     <t>LOW-POWER HIGH-ACCURACY ANALOG O</t>
@@ -138,7 +135,7 @@
     <t>Manufacturer Part Number 1</t>
   </si>
   <si>
-    <t>CC0402MRX5R6BB104</t>
+    <t>GRM155R71H104KE14J</t>
   </si>
   <si>
     <t>GRM188R60J106ME47D</t>
@@ -150,9 +147,15 @@
     <t>GRM21BR61E106KA73K</t>
   </si>
   <si>
+    <t>CL10B104KA8NNNC</t>
+  </si>
+  <si>
     <t>CL21A475KAQNNNG</t>
   </si>
   <si>
+    <t>GRM1885C1H102JA01D</t>
+  </si>
+  <si>
     <t>CC0402KRX7R7BB103</t>
   </si>
   <si>
@@ -165,18 +168,21 @@
     <t>C0402C220K5GACTU</t>
   </si>
   <si>
-    <t>CC0201KRX5R8BB102</t>
-  </si>
-  <si>
     <t>CC0603KRX7R9BB681</t>
   </si>
   <si>
+    <t>150060RS75000</t>
+  </si>
+  <si>
     <t>HK10051N8S-T</t>
   </si>
   <si>
     <t>0402HP-470EGTS</t>
   </si>
   <si>
+    <t>RC0603JR-07470RL</t>
+  </si>
+  <si>
     <t>RC0402FR-0710KL</t>
   </si>
   <si>
@@ -198,12 +204,6 @@
     <t>RC0402JR-070RL</t>
   </si>
   <si>
-    <t>RC0402FR-0760R4L</t>
-  </si>
-  <si>
-    <t>MSP432E401YTPDTR</t>
-  </si>
-  <si>
     <t>FC-13532.7680KA-AC3</t>
   </si>
   <si>
@@ -246,12 +246,12 @@
     <t>PULS-HX1188FNL-SMT-16_V</t>
   </si>
   <si>
-    <t>DBV0006A_L</t>
-  </si>
-  <si>
     <t>SOT-323_DIO</t>
   </si>
   <si>
+    <t>SOIC-SO18_L</t>
+  </si>
+  <si>
     <t>D0008A_N</t>
   </si>
   <si>
@@ -282,6 +282,9 @@
     <t>4.7uF</t>
   </si>
   <si>
+    <t>1nF</t>
+  </si>
+  <si>
     <t>10nF</t>
   </si>
   <si>
@@ -298,9 +301,6 @@
   </si>
   <si>
     <t>22pF</t>
-  </si>
-  <si>
-    <t>1nF</t>
   </si>
   <si>
     <t>680pF</t>
@@ -719,7 +719,7 @@
         <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>57</v>
@@ -765,10 +765,10 @@
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>59</v>
@@ -777,10 +777,10 @@
         <v>77</v>
       </c>
       <c r="G3">
-        <v>9.7000000000000003E-3</v>
+        <v>3.1E-2</v>
       </c>
       <c r="H3">
-        <v>0.16489999999999999</v>
+        <v>0.434</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -791,7 +791,7 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -817,7 +817,7 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -843,7 +843,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -869,22 +869,22 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G7">
-        <v>9.6000000000000002E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="H7">
-        <v>9.6000000000000002E-2</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -895,22 +895,22 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G8">
-        <v>6.0000000000000001E-3</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="H8">
-        <v>1.2E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -921,7 +921,7 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -930,13 +930,13 @@
         <v>61</v>
       </c>
       <c r="F9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G9">
-        <v>8.0000000000000002E-3</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="H9">
-        <v>8.0000000000000002E-3</v>
+        <v>4.9000000000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -947,22 +947,22 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G10">
-        <v>9.8000000000000004E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H10">
-        <v>0.19600000000000001</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -976,19 +976,19 @@
         <v>41</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G11">
-        <v>2.58E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H11">
-        <v>0.1032</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -998,23 +998,23 @@
       <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="C12">
-        <v>885012208079</v>
+      <c r="C12" t="s">
+        <v>34</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G12">
-        <v>0.12</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="H12">
-        <v>0.12</v>
+        <v>0.19600000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1028,19 +1028,19 @@
         <v>42</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" t="s">
         <v>59</v>
       </c>
       <c r="F13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G13">
-        <v>2E-3</v>
+        <v>2.58E-2</v>
       </c>
       <c r="H13">
-        <v>0.01</v>
+        <v>0.1032</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1050,23 +1050,23 @@
       <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
-        <v>43</v>
+      <c r="C14">
+        <v>885012208079</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G14">
-        <v>2.4799999999999999E-2</v>
+        <v>0.12</v>
       </c>
       <c r="H14">
-        <v>4.9599999999999998E-2</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1077,102 +1077,111 @@
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G15">
-        <v>4.3900000000000002E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="H15">
-        <v>4.3900000000000002E-2</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
         <v>61</v>
       </c>
+      <c r="F16" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16">
+        <v>4.3900000000000002E-2</v>
+      </c>
+      <c r="H16">
+        <v>4.3900000000000002E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G17">
-        <v>1.25</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H17">
-        <v>1.25</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G18">
-        <v>9.11</v>
+        <v>1.25</v>
       </c>
       <c r="H18">
-        <v>9.11</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="G19">
-        <v>2.18E-2</v>
+        <v>9.11</v>
       </c>
       <c r="H19">
-        <v>2.18E-2</v>
+        <v>9.11</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1186,59 +1195,68 @@
         <v>46</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
         <v>59</v>
       </c>
       <c r="F20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G20">
-        <v>0.24</v>
+        <v>2.18E-2</v>
       </c>
       <c r="H20">
-        <v>0.48</v>
+        <v>2.18E-2</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="F21" t="s">
+        <v>91</v>
       </c>
       <c r="G21">
-        <v>2.87</v>
+        <v>0.24</v>
       </c>
       <c r="H21">
-        <v>2.87</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22">
-        <v>470</v>
+        <v>65</v>
+      </c>
+      <c r="G22">
+        <v>2.7</v>
+      </c>
+      <c r="H22">
+        <v>2.7</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1249,22 +1267,22 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D23">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" t="s">
-        <v>92</v>
+        <v>61</v>
+      </c>
+      <c r="F23">
+        <v>470</v>
       </c>
       <c r="G23">
-        <v>3.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H23">
-        <v>1.7999999999999999E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1275,22 +1293,22 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
         <v>59</v>
       </c>
       <c r="F24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G24">
-        <v>0.38</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H24">
-        <v>0.38</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1301,22 +1319,22 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
         <v>59</v>
       </c>
-      <c r="F25">
-        <v>50</v>
+      <c r="F25" t="s">
+        <v>93</v>
       </c>
       <c r="G25">
-        <v>4.0000000000000001E-3</v>
+        <v>0.38</v>
       </c>
       <c r="H25">
-        <v>1.6E-2</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1327,22 +1345,22 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E26" t="s">
         <v>59</v>
       </c>
-      <c r="F26" t="s">
-        <v>94</v>
+      <c r="F26">
+        <v>50</v>
       </c>
       <c r="G26">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="H26">
-        <v>4.0000000000000001E-3</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1353,22 +1371,22 @@
         <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
         <v>59</v>
       </c>
-      <c r="F27">
-        <v>75</v>
+      <c r="F27" t="s">
+        <v>94</v>
       </c>
       <c r="G27">
-        <v>3.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H27">
-        <v>1.2E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1379,22 +1397,22 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" t="s">
-        <v>95</v>
+        <v>59</v>
+      </c>
+      <c r="F28">
+        <v>75</v>
       </c>
       <c r="G28">
-        <v>9.8000000000000004E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H28">
-        <v>9.8000000000000004E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1405,22 +1423,22 @@
         <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="F29" t="s">
+        <v>95</v>
       </c>
       <c r="G29">
-        <v>2E-3</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="H29">
-        <v>6.0000000000000001E-3</v>
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1431,7 +1449,7 @@
         <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -1440,13 +1458,13 @@
         <v>59</v>
       </c>
       <c r="F30">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>1.2E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="H30">
-        <v>0.12</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1502,9 +1520,6 @@
       <c r="B33" t="s">
         <v>25</v>
       </c>
-      <c r="C33" t="s">
-        <v>55</v>
-      </c>
       <c r="D33">
         <v>1</v>
       </c>
@@ -1513,12 +1528,6 @@
       </c>
       <c r="F33" t="s">
         <v>76</v>
-      </c>
-      <c r="G33">
-        <v>15.45</v>
-      </c>
-      <c r="H33">
-        <v>15.45</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1538,16 +1547,19 @@
         <v>69</v>
       </c>
       <c r="G34">
-        <v>4.8499999999999996</v>
+        <v>4.08</v>
       </c>
       <c r="H34">
-        <v>4.8499999999999996</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
       <c r="C35" t="s">
         <v>13</v>
       </c>
@@ -1555,36 +1567,33 @@
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="G35">
-        <v>14.16</v>
+        <v>0.2301</v>
       </c>
       <c r="H35">
-        <v>14.16</v>
+        <v>0.2301</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
-      <c r="B36" t="s">
-        <v>28</v>
-      </c>
       <c r="C36" t="s">
         <v>14</v>
       </c>
       <c r="D36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="G36">
-        <v>0.15035000000000001</v>
+        <v>14.16</v>
       </c>
       <c r="H36">
-        <v>0.30070000000000002</v>
+        <v>14.16</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1592,7 +1601,7 @@
         <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
         <v>15</v>
@@ -1604,10 +1613,10 @@
         <v>71</v>
       </c>
       <c r="G37">
-        <v>0.2301</v>
+        <v>1.78</v>
       </c>
       <c r="H37">
-        <v>0.2301</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1615,7 +1624,7 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C38" t="s">
         <v>16</v>
@@ -1626,11 +1635,14 @@
       <c r="E38" t="s">
         <v>72</v>
       </c>
+      <c r="F38" t="s">
+        <v>76</v>
+      </c>
       <c r="G38">
-        <v>1.28</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H38">
-        <v>1.28</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1638,7 +1650,7 @@
         <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
@@ -1661,7 +1673,7 @@
         <v>18</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C40" t="s">
         <v>56</v>
@@ -1678,7 +1690,7 @@
         <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C41" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Fixed all errors found by manually reviewing the master BOM
</commit_message>
<xml_diff>
--- a/ACDC/Project Outputs for ACDC/ACDC.xlsx
+++ b/ACDC/Project Outputs for ACDC/ACDC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr3de\Documents\MASA\2020-21-PCBs\ACDC\Project Outputs for ACDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17D81DEC-9BB3-4ACB-A4FB-63C7F14EA9E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A761CC3-4543-49AB-817B-75B57BDF6BFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{D24AC2E5-4D69-4F47-9D68-7C6EF3866D9C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -138,9 +138,6 @@
     <t>GRM155R71H104KE14J</t>
   </si>
   <si>
-    <t>GRM188R60J106ME47D</t>
-  </si>
-  <si>
     <t>0402B682K500CT</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
     <t>CL10B105MO8NNWC</t>
   </si>
   <si>
+    <t>GRM188R61E225KA12D</t>
+  </si>
+  <si>
     <t>CC0402JRNPO9BN120</t>
   </si>
   <si>
@@ -268,9 +268,6 @@
   </si>
   <si>
     <t>100nF</t>
-  </si>
-  <si>
-    <t>120nF</t>
   </si>
   <si>
     <t>6.8nF</t>
@@ -703,7 +700,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A74CBD-EB5E-4691-BC08-A422B7428F5D}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
@@ -731,10 +728,10 @@
         <v>76</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -768,7 +765,7 @@
         <v>33</v>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>59</v>
@@ -780,7 +777,7 @@
         <v>3.1E-2</v>
       </c>
       <c r="H3">
-        <v>0.434</v>
+        <v>0.496</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -803,10 +800,10 @@
         <v>78</v>
       </c>
       <c r="G4">
-        <v>9.8000000000000004E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="H4">
-        <v>0.19600000000000001</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -820,19 +817,19 @@
         <v>35</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
         <v>79</v>
       </c>
       <c r="G5">
-        <v>1E-3</v>
+        <v>0.16350000000000001</v>
       </c>
       <c r="H5">
-        <v>2E-3</v>
+        <v>0.16350000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -846,19 +843,19 @@
         <v>36</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G6">
-        <v>0.16350000000000001</v>
+        <v>2.7E-2</v>
       </c>
       <c r="H6">
-        <v>0.16350000000000001</v>
+        <v>0.27</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -872,19 +869,19 @@
         <v>37</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="G7">
-        <v>2.7E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="H7">
-        <v>0.27</v>
+        <v>9.6000000000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -901,16 +898,16 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F8" t="s">
         <v>81</v>
       </c>
       <c r="G8">
-        <v>9.6000000000000002E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H8">
-        <v>9.6000000000000002E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -924,19 +921,19 @@
         <v>39</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
         <v>82</v>
       </c>
       <c r="G9">
-        <v>4.9000000000000002E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H9">
-        <v>4.9000000000000002E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -950,19 +947,19 @@
         <v>40</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
         <v>83</v>
       </c>
       <c r="G10">
-        <v>6.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="H10">
-        <v>1.2E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -976,7 +973,7 @@
         <v>41</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="s">
         <v>61</v>
@@ -985,10 +982,10 @@
         <v>84</v>
       </c>
       <c r="G11">
-        <v>8.0000000000000002E-3</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="H11">
-        <v>8.0000000000000002E-3</v>
+        <v>0.20399999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -999,22 +996,22 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F12" t="s">
         <v>85</v>
       </c>
       <c r="G12">
-        <v>9.8000000000000004E-2</v>
+        <v>2.58E-2</v>
       </c>
       <c r="H12">
-        <v>0.19600000000000001</v>
+        <v>0.1032</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1024,23 +1021,23 @@
       <c r="B13" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="s">
-        <v>42</v>
+      <c r="C13">
+        <v>885012208079</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
         <v>86</v>
       </c>
       <c r="G13">
-        <v>2.58E-2</v>
+        <v>0.12</v>
       </c>
       <c r="H13">
-        <v>0.1032</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1050,23 +1047,23 @@
       <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="C14">
-        <v>885012208079</v>
+      <c r="C14" t="s">
+        <v>43</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
         <v>87</v>
       </c>
       <c r="G14">
-        <v>0.12</v>
+        <v>2E-3</v>
       </c>
       <c r="H14">
-        <v>0.12</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1077,111 +1074,111 @@
         <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F15" t="s">
         <v>88</v>
       </c>
       <c r="G15">
-        <v>2E-3</v>
+        <v>4.3900000000000002E-2</v>
       </c>
       <c r="H15">
-        <v>0.01</v>
+        <v>4.3900000000000002E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
         <v>61</v>
       </c>
-      <c r="F16" t="s">
-        <v>89</v>
-      </c>
       <c r="G16">
-        <v>4.3900000000000002E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H16">
-        <v>4.3900000000000002E-2</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G17">
-        <v>0.14000000000000001</v>
+        <v>1.25</v>
       </c>
       <c r="H17">
-        <v>0.42</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G18">
-        <v>1.25</v>
+        <v>9.11</v>
       </c>
       <c r="H18">
-        <v>1.25</v>
+        <v>9.11</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+      <c r="F19" t="s">
+        <v>89</v>
       </c>
       <c r="G19">
-        <v>9.11</v>
+        <v>2.18E-2</v>
       </c>
       <c r="H19">
-        <v>9.11</v>
+        <v>2.18E-2</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1192,10 +1189,10 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
         <v>59</v>
@@ -1204,59 +1201,59 @@
         <v>90</v>
       </c>
       <c r="G20">
-        <v>2.18E-2</v>
+        <v>0.24</v>
       </c>
       <c r="H20">
-        <v>2.18E-2</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="G21">
-        <v>0.24</v>
+        <v>2.7</v>
       </c>
       <c r="H21">
-        <v>0.48</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>61</v>
+      </c>
+      <c r="F22">
+        <v>470</v>
       </c>
       <c r="G22">
-        <v>2.7</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H22">
-        <v>2.7</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1267,22 +1264,22 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23">
-        <v>470</v>
+        <v>59</v>
+      </c>
+      <c r="F23" t="s">
+        <v>91</v>
       </c>
       <c r="G23">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H23">
-        <v>1.2E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1293,10 +1290,10 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E24" t="s">
         <v>59</v>
@@ -1305,10 +1302,10 @@
         <v>92</v>
       </c>
       <c r="G24">
-        <v>3.0000000000000001E-3</v>
+        <v>0.38</v>
       </c>
       <c r="H24">
-        <v>1.4999999999999999E-2</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1319,22 +1316,22 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E25" t="s">
         <v>59</v>
       </c>
-      <c r="F25" t="s">
-        <v>93</v>
+      <c r="F25">
+        <v>50</v>
       </c>
       <c r="G25">
-        <v>0.38</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H25">
-        <v>0.38</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1345,22 +1342,22 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>59</v>
       </c>
-      <c r="F26">
-        <v>50</v>
+      <c r="F26" t="s">
+        <v>93</v>
       </c>
       <c r="G26">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="H26">
-        <v>1.6E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1371,22 +1368,22 @@
         <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E27" t="s">
         <v>59</v>
       </c>
-      <c r="F27" t="s">
-        <v>94</v>
+      <c r="F27">
+        <v>75</v>
       </c>
       <c r="G27">
-        <v>4.0000000000000001E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H27">
-        <v>4.0000000000000001E-3</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1397,22 +1394,22 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D28">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
-      </c>
-      <c r="F28">
-        <v>75</v>
+        <v>62</v>
+      </c>
+      <c r="F28" t="s">
+        <v>94</v>
       </c>
       <c r="G28">
-        <v>3.0000000000000001E-3</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="H28">
-        <v>1.2E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1423,289 +1420,272 @@
         <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" t="s">
-        <v>95</v>
+        <v>59</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
       </c>
       <c r="G29">
-        <v>9.8000000000000004E-2</v>
+        <v>2E-3</v>
       </c>
       <c r="H29">
-        <v>9.8000000000000004E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="G30">
-        <v>2E-3</v>
+        <v>0.13</v>
       </c>
       <c r="H30">
-        <v>4.0000000000000001E-3</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G31">
-        <v>0.13</v>
+        <v>10.06</v>
       </c>
       <c r="H31">
-        <v>0.13</v>
+        <v>20.12</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="F32" t="s">
+        <v>76</v>
       </c>
       <c r="G32">
-        <v>10.06</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="H32">
-        <v>20.12</v>
+        <v>16.600000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+      <c r="G33">
+        <v>4.08</v>
+      </c>
+      <c r="H33">
+        <v>4.08</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G34">
-        <v>4.08</v>
+        <v>0.2301</v>
       </c>
       <c r="H34">
-        <v>4.08</v>
+        <v>0.2301</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="G35">
-        <v>0.2301</v>
+        <v>14.16</v>
       </c>
       <c r="H35">
-        <v>0.2301</v>
+        <v>14.16</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="G36">
-        <v>14.16</v>
+        <v>1.78</v>
       </c>
       <c r="H36">
-        <v>14.16</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="F37" t="s">
+        <v>76</v>
       </c>
       <c r="G37">
-        <v>1.78</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H37">
-        <v>1.78</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>72</v>
-      </c>
-      <c r="F38" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G38">
-        <v>2.2999999999999998</v>
+        <v>0.75839999999999996</v>
       </c>
       <c r="H38">
-        <v>2.2999999999999998</v>
+        <v>0.75839999999999996</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B39" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>73</v>
-      </c>
-      <c r="G39">
-        <v>0.75839999999999996</v>
-      </c>
-      <c r="H39">
-        <v>0.75839999999999996</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
         <v>75</v>
       </c>
-      <c r="G41">
-        <v>0.83799999999999997</v>
-      </c>
-      <c r="H41">
-        <v>0.83799999999999997</v>
+      <c r="G40">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="H40">
+        <v>0.81299999999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got all BOMs up to date
</commit_message>
<xml_diff>
--- a/ACDC/Project Outputs for ACDC/ACDC.xlsx
+++ b/ACDC/Project Outputs for ACDC/ACDC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr3de\Documents\MASA\2020-21-PCBs\ACDC\Project Outputs for ACDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A761CC3-4543-49AB-817B-75B57BDF6BFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{83AFC687-6C5E-46E2-8B1B-4C4AEFD87491}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{D24AC2E5-4D69-4F47-9D68-7C6EF3866D9C}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{D24AC2E5-4D69-4F47-9D68-7C6EF3866D9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -803,7 +803,7 @@
         <v>1E-3</v>
       </c>
       <c r="H4">
-        <v>2E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -852,10 +852,10 @@
         <v>77</v>
       </c>
       <c r="G6">
-        <v>2.7E-2</v>
+        <v>2.5700000000000001E-2</v>
       </c>
       <c r="H6">
-        <v>0.27</v>
+        <v>0.25700000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -904,10 +904,10 @@
         <v>81</v>
       </c>
       <c r="G8">
-        <v>8.0000000000000002E-3</v>
+        <v>4.8300000000000003E-2</v>
       </c>
       <c r="H8">
-        <v>8.0000000000000002E-3</v>
+        <v>4.8300000000000003E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -930,10 +930,10 @@
         <v>82</v>
       </c>
       <c r="G9">
-        <v>6.0000000000000001E-3</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H9">
-        <v>1.2E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -956,10 +956,10 @@
         <v>83</v>
       </c>
       <c r="G10">
-        <v>8.0000000000000002E-3</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="H10">
-        <v>8.0000000000000002E-3</v>
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -982,10 +982,10 @@
         <v>84</v>
       </c>
       <c r="G11">
-        <v>0.10199999999999999</v>
+        <v>0.10589999999999999</v>
       </c>
       <c r="H11">
-        <v>0.20399999999999999</v>
+        <v>0.21179999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1060,10 +1060,10 @@
         <v>87</v>
       </c>
       <c r="G14">
-        <v>2E-3</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="H14">
-        <v>0.01</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1224,10 +1224,10 @@
         <v>65</v>
       </c>
       <c r="G21">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="H21">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1250,10 +1250,10 @@
         <v>470</v>
       </c>
       <c r="G22">
-        <v>4.0000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="H22">
-        <v>1.2E-2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1276,10 +1276,10 @@
         <v>91</v>
       </c>
       <c r="G23">
-        <v>3.0000000000000001E-3</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H23">
-        <v>1.4999999999999999E-2</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1328,10 +1328,10 @@
         <v>50</v>
       </c>
       <c r="G25">
-        <v>4.0000000000000001E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="H25">
-        <v>1.6E-2</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1354,10 +1354,10 @@
         <v>93</v>
       </c>
       <c r="G26">
-        <v>4.0000000000000001E-3</v>
+        <v>2.4E-2</v>
       </c>
       <c r="H26">
-        <v>4.0000000000000001E-3</v>
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1380,10 +1380,10 @@
         <v>75</v>
       </c>
       <c r="G27">
-        <v>3.0000000000000001E-3</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H27">
-        <v>1.2E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1432,10 +1432,10 @@
         <v>0</v>
       </c>
       <c r="G29">
-        <v>2E-3</v>
+        <v>0.01</v>
       </c>
       <c r="H29">
-        <v>4.0000000000000001E-3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1527,10 +1527,10 @@
         <v>69</v>
       </c>
       <c r="G33">
-        <v>4.08</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="H33">
-        <v>4.08</v>
+        <v>4.8499999999999996</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1593,10 +1593,10 @@
         <v>71</v>
       </c>
       <c r="G36">
-        <v>1.78</v>
+        <v>1.71</v>
       </c>
       <c r="H36">
-        <v>1.78</v>
+        <v>1.71</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1664,6 +1664,12 @@
       <c r="E39" t="s">
         <v>74</v>
       </c>
+      <c r="G39">
+        <v>0.41</v>
+      </c>
+      <c r="H39">
+        <v>0.41</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1682,10 +1688,10 @@
         <v>75</v>
       </c>
       <c r="G40">
-        <v>0.81299999999999994</v>
+        <v>0.95330000000000004</v>
       </c>
       <c r="H40">
-        <v>0.81299999999999994</v>
+        <v>0.95330000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed BPDC and did master BOM
</commit_message>
<xml_diff>
--- a/ACDC/Project Outputs for ACDC/ACDC.xlsx
+++ b/ACDC/Project Outputs for ACDC/ACDC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr3de\Documents\MASA\2020-21-PCBs\ACDC\Project Outputs for ACDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83AFC687-6C5E-46E2-8B1B-4C4AEFD87491}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10B86081-5A70-4E54-8446-465B5B2B1F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{D24AC2E5-4D69-4F47-9D68-7C6EF3866D9C}"/>
+    <workbookView xWindow="3720" yWindow="3720" windowWidth="21600" windowHeight="11385" xr2:uid="{D24AC2E5-4D69-4F47-9D68-7C6EF3866D9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -75,18 +75,15 @@
     <t>HX1188FNL</t>
   </si>
   <si>
+    <t>M20048-1</t>
+  </si>
+  <si>
+    <t>TCAN334DR</t>
+  </si>
+  <si>
     <t>D5V0L2B3W-7</t>
   </si>
   <si>
-    <t>M20048-1</t>
-  </si>
-  <si>
-    <t>MCP2515-I/SO</t>
-  </si>
-  <si>
-    <t>TCAN334DR</t>
-  </si>
-  <si>
     <t>TMP235A2DBZR</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>Telecom Transformer 1:1/1:1, -40 to 85 degC, 16-Pin SMT, RoHS, Tube</t>
   </si>
   <si>
-    <t>Stand-Alone CAN Controller With SPI Interface, 18-Pin SOIC, Industrial Temperature</t>
-  </si>
-  <si>
     <t>LOW-POWER HIGH-ACCURACY ANALOG O</t>
   </si>
   <si>
@@ -144,30 +138,33 @@
     <t>GRM21BR61E106KA73K</t>
   </si>
   <si>
+    <t>CL21A475KAQNNNG</t>
+  </si>
+  <si>
+    <t>CC0402KRX7R7BB103</t>
+  </si>
+  <si>
+    <t>CL10B105MO8NNWC</t>
+  </si>
+  <si>
+    <t>GRM188R61E225KA12D</t>
+  </si>
+  <si>
+    <t>CC0402JRNPO9BN120</t>
+  </si>
+  <si>
+    <t>C0402C220K5GACTU</t>
+  </si>
+  <si>
+    <t>CL05A225KA5NUNC</t>
+  </si>
+  <si>
     <t>CL10B104KA8NNNC</t>
   </si>
   <si>
-    <t>CL21A475KAQNNNG</t>
-  </si>
-  <si>
     <t>GRM1885C1H102JA01D</t>
   </si>
   <si>
-    <t>CC0402KRX7R7BB103</t>
-  </si>
-  <si>
-    <t>CL10B105MO8NNWC</t>
-  </si>
-  <si>
-    <t>GRM188R61E225KA12D</t>
-  </si>
-  <si>
-    <t>CC0402JRNPO9BN120</t>
-  </si>
-  <si>
-    <t>C0402C220K5GACTU</t>
-  </si>
-  <si>
     <t>CC0603KRX7R9BB681</t>
   </si>
   <si>
@@ -246,15 +243,12 @@
     <t>PULS-HX1188FNL-SMT-16_V</t>
   </si>
   <si>
+    <t>D0008A_N</t>
+  </si>
+  <si>
     <t>SOT-323_DIO</t>
   </si>
   <si>
-    <t>SOIC-SO18_L</t>
-  </si>
-  <si>
-    <t>D0008A_N</t>
-  </si>
-  <si>
     <t>FP-DBZ0003A-MFG</t>
   </si>
   <si>
@@ -279,25 +273,25 @@
     <t>4.7uF</t>
   </si>
   <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>12pF</t>
+  </si>
+  <si>
+    <t>4.7nF</t>
+  </si>
+  <si>
+    <t>22pF</t>
+  </si>
+  <si>
     <t>1nF</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
-    <t>12pF</t>
-  </si>
-  <si>
-    <t>4.7nF</t>
-  </si>
-  <si>
-    <t>22pF</t>
   </si>
   <si>
     <t>680pF</t>
@@ -713,25 +707,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -748,10 +742,10 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>2.04</v>
+        <v>2.14</v>
       </c>
       <c r="H2">
-        <v>2.04</v>
+        <v>2.14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -759,25 +753,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G3">
-        <v>3.1E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H3">
-        <v>0.496</v>
+        <v>0.35199999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -785,19 +779,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G4">
         <v>1E-3</v>
@@ -811,25 +805,25 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G5">
-        <v>0.16350000000000001</v>
+        <v>7.3700000000000002E-2</v>
       </c>
       <c r="H5">
-        <v>0.16350000000000001</v>
+        <v>7.3700000000000002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -837,25 +831,25 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G6">
-        <v>2.5700000000000001E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="H6">
-        <v>0.25700000000000001</v>
+        <v>9.6000000000000002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -863,25 +857,25 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G7">
-        <v>9.6000000000000002E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H7">
-        <v>9.6000000000000002E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -889,25 +883,25 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G8">
-        <v>4.8300000000000003E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="H8">
-        <v>4.8300000000000003E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -915,25 +909,25 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G9">
-        <v>2.1000000000000001E-2</v>
+        <v>0.1036</v>
       </c>
       <c r="H9">
-        <v>4.2000000000000003E-2</v>
+        <v>0.1036</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -941,25 +935,25 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G10">
-        <v>9.8000000000000004E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="H10">
-        <v>9.8000000000000004E-2</v>
+        <v>2.1600000000000001E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -967,25 +961,25 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>885012208079</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G11">
-        <v>0.10589999999999999</v>
+        <v>0.12</v>
       </c>
       <c r="H11">
-        <v>0.21179999999999999</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -993,25 +987,25 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G12">
-        <v>2.58E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="H12">
-        <v>0.1032</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1019,25 +1013,25 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13">
-        <v>885012208079</v>
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F13" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G13">
-        <v>0.12</v>
+        <v>0.35</v>
       </c>
       <c r="H13">
-        <v>0.12</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1045,25 +1039,25 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="G14">
-        <v>1.0999999999999999E-2</v>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="H14">
-        <v>0.11</v>
+        <v>2.3099999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1071,114 +1065,114 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G15">
-        <v>4.3900000000000002E-2</v>
+        <v>1.44E-2</v>
       </c>
       <c r="H15">
-        <v>4.3900000000000002E-2</v>
+        <v>1.44E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="F16" t="s">
+        <v>86</v>
       </c>
       <c r="G16">
-        <v>0.14000000000000001</v>
+        <v>1.0699999999999999E-2</v>
       </c>
       <c r="H16">
-        <v>0.42</v>
+        <v>1.0699999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G17">
-        <v>1.25</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H17">
-        <v>1.25</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G18">
-        <v>9.11</v>
+        <v>1.25</v>
       </c>
       <c r="H18">
-        <v>9.11</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="G19">
-        <v>2.18E-2</v>
+        <v>9.11</v>
       </c>
       <c r="H19">
-        <v>2.18E-2</v>
+        <v>9.11</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1189,71 +1183,71 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G20">
-        <v>0.24</v>
+        <v>2.18E-2</v>
       </c>
       <c r="H20">
-        <v>0.48</v>
+        <v>2.18E-2</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>58</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
       </c>
       <c r="G21">
-        <v>2.5</v>
+        <v>0.24</v>
       </c>
       <c r="H21">
-        <v>2.5</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22">
-        <v>470</v>
+        <v>64</v>
       </c>
       <c r="G22">
-        <v>1.4999999999999999E-2</v>
+        <v>2.61</v>
       </c>
       <c r="H22">
-        <v>0.15</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1261,25 +1255,25 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" t="s">
-        <v>91</v>
+        <v>60</v>
+      </c>
+      <c r="F23">
+        <v>470</v>
       </c>
       <c r="G23">
-        <v>1.2999999999999999E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="H23">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1287,25 +1281,25 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G24">
-        <v>0.38</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H24">
-        <v>0.38</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1313,25 +1307,25 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25">
-        <v>50</v>
+        <v>58</v>
+      </c>
+      <c r="F25" t="s">
+        <v>90</v>
       </c>
       <c r="G25">
-        <v>1.2E-2</v>
+        <v>0.38</v>
       </c>
       <c r="H25">
-        <v>0.12</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1339,25 +1333,25 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" t="s">
-        <v>93</v>
+        <v>58</v>
+      </c>
+      <c r="F26">
+        <v>50</v>
       </c>
       <c r="G26">
-        <v>2.4E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="H26">
-        <v>2.4E-2</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1365,25 +1359,25 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27">
-        <v>75</v>
+        <v>58</v>
+      </c>
+      <c r="F27" t="s">
+        <v>91</v>
       </c>
       <c r="G27">
-        <v>1.2999999999999999E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H27">
-        <v>5.1999999999999998E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1391,25 +1385,25 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" t="s">
-        <v>94</v>
+        <v>58</v>
+      </c>
+      <c r="F28">
+        <v>75</v>
       </c>
       <c r="G28">
-        <v>9.8000000000000004E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H28">
-        <v>9.8000000000000004E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1417,229 +1411,226 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
+        <v>61</v>
+      </c>
+      <c r="F29" t="s">
+        <v>92</v>
       </c>
       <c r="G29">
-        <v>0.01</v>
+        <v>9.1000000000000004E-3</v>
       </c>
       <c r="H29">
-        <v>0.1</v>
+        <v>9.1000000000000004E-3</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>58</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>0.13</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="H30">
-        <v>0.13</v>
+        <v>3.2000000000000002E-3</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G31">
-        <v>10.06</v>
+        <v>0.13</v>
       </c>
       <c r="H31">
-        <v>20.12</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
         <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>68</v>
-      </c>
-      <c r="F32" t="s">
-        <v>76</v>
-      </c>
-      <c r="G32">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="H32">
-        <v>16.600000000000001</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="F33" t="s">
+        <v>74</v>
       </c>
       <c r="G33">
-        <v>4.8499999999999996</v>
+        <v>10.51</v>
       </c>
       <c r="H33">
-        <v>4.8499999999999996</v>
+        <v>10.51</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G34">
-        <v>0.2301</v>
+        <v>3.64</v>
       </c>
       <c r="H34">
-        <v>0.2301</v>
+        <v>3.64</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35">
-        <v>14.16</v>
+        <v>14.66</v>
       </c>
       <c r="H35">
-        <v>14.16</v>
+        <v>14.66</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+      <c r="F36" t="s">
+        <v>74</v>
       </c>
       <c r="G36">
-        <v>1.71</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H36">
-        <v>1.71</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>72</v>
-      </c>
-      <c r="F37" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G37">
-        <v>2.2999999999999998</v>
+        <v>0.2301</v>
       </c>
       <c r="H37">
-        <v>2.2999999999999998</v>
+        <v>0.2301</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G38">
         <v>0.75839999999999996</v>
@@ -1650,42 +1641,36 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
-      </c>
-      <c r="G39">
-        <v>0.41</v>
-      </c>
-      <c r="H39">
-        <v>0.41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G40">
         <v>0.95330000000000004</v>

</xml_diff>

<commit_message>
Routed ethernet and fixed ethernet symbol
</commit_message>
<xml_diff>
--- a/ACDC/Project Outputs for ACDC/ACDC.xlsx
+++ b/ACDC/Project Outputs for ACDC/ACDC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pr3de\Documents\MASA\2020-21-PCBs\ACDC\Project Outputs for ACDC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83AFC687-6C5E-46E2-8B1B-4C4AEFD87491}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10B86081-5A70-4E54-8446-465B5B2B1F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{D24AC2E5-4D69-4F47-9D68-7C6EF3866D9C}"/>
+    <workbookView xWindow="3720" yWindow="3720" windowWidth="21600" windowHeight="11385" xr2:uid="{D24AC2E5-4D69-4F47-9D68-7C6EF3866D9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -75,18 +75,15 @@
     <t>HX1188FNL</t>
   </si>
   <si>
+    <t>M20048-1</t>
+  </si>
+  <si>
+    <t>TCAN334DR</t>
+  </si>
+  <si>
     <t>D5V0L2B3W-7</t>
   </si>
   <si>
-    <t>M20048-1</t>
-  </si>
-  <si>
-    <t>MCP2515-I/SO</t>
-  </si>
-  <si>
-    <t>TCAN334DR</t>
-  </si>
-  <si>
     <t>TMP235A2DBZR</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>Telecom Transformer 1:1/1:1, -40 to 85 degC, 16-Pin SMT, RoHS, Tube</t>
   </si>
   <si>
-    <t>Stand-Alone CAN Controller With SPI Interface, 18-Pin SOIC, Industrial Temperature</t>
-  </si>
-  <si>
     <t>LOW-POWER HIGH-ACCURACY ANALOG O</t>
   </si>
   <si>
@@ -144,30 +138,33 @@
     <t>GRM21BR61E106KA73K</t>
   </si>
   <si>
+    <t>CL21A475KAQNNNG</t>
+  </si>
+  <si>
+    <t>CC0402KRX7R7BB103</t>
+  </si>
+  <si>
+    <t>CL10B105MO8NNWC</t>
+  </si>
+  <si>
+    <t>GRM188R61E225KA12D</t>
+  </si>
+  <si>
+    <t>CC0402JRNPO9BN120</t>
+  </si>
+  <si>
+    <t>C0402C220K5GACTU</t>
+  </si>
+  <si>
+    <t>CL05A225KA5NUNC</t>
+  </si>
+  <si>
     <t>CL10B104KA8NNNC</t>
   </si>
   <si>
-    <t>CL21A475KAQNNNG</t>
-  </si>
-  <si>
     <t>GRM1885C1H102JA01D</t>
   </si>
   <si>
-    <t>CC0402KRX7R7BB103</t>
-  </si>
-  <si>
-    <t>CL10B105MO8NNWC</t>
-  </si>
-  <si>
-    <t>GRM188R61E225KA12D</t>
-  </si>
-  <si>
-    <t>CC0402JRNPO9BN120</t>
-  </si>
-  <si>
-    <t>C0402C220K5GACTU</t>
-  </si>
-  <si>
     <t>CC0603KRX7R9BB681</t>
   </si>
   <si>
@@ -246,15 +243,12 @@
     <t>PULS-HX1188FNL-SMT-16_V</t>
   </si>
   <si>
+    <t>D0008A_N</t>
+  </si>
+  <si>
     <t>SOT-323_DIO</t>
   </si>
   <si>
-    <t>SOIC-SO18_L</t>
-  </si>
-  <si>
-    <t>D0008A_N</t>
-  </si>
-  <si>
     <t>FP-DBZ0003A-MFG</t>
   </si>
   <si>
@@ -279,25 +273,25 @@
     <t>4.7uF</t>
   </si>
   <si>
+    <t>10nF</t>
+  </si>
+  <si>
+    <t>1uF</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>12pF</t>
+  </si>
+  <si>
+    <t>4.7nF</t>
+  </si>
+  <si>
+    <t>22pF</t>
+  </si>
+  <si>
     <t>1nF</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>1uF</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
-    <t>12pF</t>
-  </si>
-  <si>
-    <t>4.7nF</t>
-  </si>
-  <si>
-    <t>22pF</t>
   </si>
   <si>
     <t>680pF</t>
@@ -713,25 +707,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -748,10 +742,10 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>2.04</v>
+        <v>2.14</v>
       </c>
       <c r="H2">
-        <v>2.04</v>
+        <v>2.14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -759,25 +753,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G3">
-        <v>3.1E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="H3">
-        <v>0.496</v>
+        <v>0.35199999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -785,19 +779,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G4">
         <v>1E-3</v>
@@ -811,25 +805,25 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G5">
-        <v>0.16350000000000001</v>
+        <v>7.3700000000000002E-2</v>
       </c>
       <c r="H5">
-        <v>0.16350000000000001</v>
+        <v>7.3700000000000002E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -837,25 +831,25 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G6">
-        <v>2.5700000000000001E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="H6">
-        <v>0.25700000000000001</v>
+        <v>9.6000000000000002E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -863,25 +857,25 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G7">
-        <v>9.6000000000000002E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H7">
-        <v>9.6000000000000002E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -889,25 +883,25 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G8">
-        <v>4.8300000000000003E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="H8">
-        <v>4.8300000000000003E-2</v>
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -915,25 +909,25 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G9">
-        <v>2.1000000000000001E-2</v>
+        <v>0.1036</v>
       </c>
       <c r="H9">
-        <v>4.2000000000000003E-2</v>
+        <v>0.1036</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -941,25 +935,25 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G10">
-        <v>9.8000000000000004E-2</v>
+        <v>5.4000000000000003E-3</v>
       </c>
       <c r="H10">
-        <v>9.8000000000000004E-2</v>
+        <v>2.1600000000000001E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -967,25 +961,25 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>885012208079</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>61</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G11">
-        <v>0.10589999999999999</v>
+        <v>0.12</v>
       </c>
       <c r="H11">
-        <v>0.21179999999999999</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -993,25 +987,25 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G12">
-        <v>2.58E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="H12">
-        <v>0.1032</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1019,25 +1013,25 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13">
-        <v>885012208079</v>
+        <v>20</v>
+      </c>
+      <c r="C13" t="s">
+        <v>40</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F13" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G13">
-        <v>0.12</v>
+        <v>0.35</v>
       </c>
       <c r="H13">
-        <v>0.12</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1045,25 +1039,25 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="G14">
-        <v>1.0999999999999999E-2</v>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="H14">
-        <v>0.11</v>
+        <v>2.3099999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1071,114 +1065,114 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F15" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G15">
-        <v>4.3900000000000002E-2</v>
+        <v>1.44E-2</v>
       </c>
       <c r="H15">
-        <v>4.3900000000000002E-2</v>
+        <v>1.44E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="F16" t="s">
+        <v>86</v>
       </c>
       <c r="G16">
-        <v>0.14000000000000001</v>
+        <v>1.0699999999999999E-2</v>
       </c>
       <c r="H16">
-        <v>0.42</v>
+        <v>1.0699999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G17">
-        <v>1.25</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H17">
-        <v>1.25</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G18">
-        <v>9.11</v>
+        <v>1.25</v>
       </c>
       <c r="H18">
-        <v>9.11</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F19" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="G19">
-        <v>2.18E-2</v>
+        <v>9.11</v>
       </c>
       <c r="H19">
-        <v>2.18E-2</v>
+        <v>9.11</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1189,71 +1183,71 @@
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G20">
-        <v>0.24</v>
+        <v>2.18E-2</v>
       </c>
       <c r="H20">
-        <v>0.48</v>
+        <v>2.18E-2</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>58</v>
+      </c>
+      <c r="F21" t="s">
+        <v>88</v>
       </c>
       <c r="G21">
-        <v>2.5</v>
+        <v>0.24</v>
       </c>
       <c r="H21">
-        <v>2.5</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22">
-        <v>470</v>
+        <v>64</v>
       </c>
       <c r="G22">
-        <v>1.4999999999999999E-2</v>
+        <v>2.61</v>
       </c>
       <c r="H22">
-        <v>0.15</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1261,25 +1255,25 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" t="s">
-        <v>91</v>
+        <v>60</v>
+      </c>
+      <c r="F23">
+        <v>470</v>
       </c>
       <c r="G23">
-        <v>1.2999999999999999E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="H23">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1287,25 +1281,25 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F24" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G24">
-        <v>0.38</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="H24">
-        <v>0.38</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1313,25 +1307,25 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25">
-        <v>50</v>
+        <v>58</v>
+      </c>
+      <c r="F25" t="s">
+        <v>90</v>
       </c>
       <c r="G25">
-        <v>1.2E-2</v>
+        <v>0.38</v>
       </c>
       <c r="H25">
-        <v>0.12</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1339,25 +1333,25 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" t="s">
-        <v>93</v>
+        <v>58</v>
+      </c>
+      <c r="F26">
+        <v>50</v>
       </c>
       <c r="G26">
-        <v>2.4E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="H26">
-        <v>2.4E-2</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1365,25 +1359,25 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
-      </c>
-      <c r="F27">
-        <v>75</v>
+        <v>58</v>
+      </c>
+      <c r="F27" t="s">
+        <v>91</v>
       </c>
       <c r="G27">
-        <v>1.2999999999999999E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="H27">
-        <v>5.1999999999999998E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1391,25 +1385,25 @@
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" t="s">
-        <v>94</v>
+        <v>58</v>
+      </c>
+      <c r="F28">
+        <v>75</v>
       </c>
       <c r="G28">
-        <v>9.8000000000000004E-2</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="H28">
-        <v>9.8000000000000004E-2</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1417,229 +1411,226 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
+        <v>61</v>
+      </c>
+      <c r="F29" t="s">
+        <v>92</v>
       </c>
       <c r="G29">
-        <v>0.01</v>
+        <v>9.1000000000000004E-3</v>
       </c>
       <c r="H29">
-        <v>0.1</v>
+        <v>9.1000000000000004E-3</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>66</v>
+        <v>58</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>0.13</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="H30">
-        <v>0.13</v>
+        <v>3.2000000000000002E-3</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G31">
-        <v>10.06</v>
+        <v>0.13</v>
       </c>
       <c r="H31">
-        <v>20.12</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
         <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
-        <v>68</v>
-      </c>
-      <c r="F32" t="s">
-        <v>76</v>
-      </c>
-      <c r="G32">
-        <v>16.600000000000001</v>
-      </c>
-      <c r="H32">
-        <v>16.600000000000001</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="F33" t="s">
+        <v>74</v>
       </c>
       <c r="G33">
-        <v>4.8499999999999996</v>
+        <v>10.51</v>
       </c>
       <c r="H33">
-        <v>4.8499999999999996</v>
+        <v>10.51</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G34">
-        <v>0.2301</v>
+        <v>3.64</v>
       </c>
       <c r="H34">
-        <v>0.2301</v>
+        <v>3.64</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G35">
-        <v>14.16</v>
+        <v>14.66</v>
       </c>
       <c r="H35">
-        <v>14.16</v>
+        <v>14.66</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+      <c r="F36" t="s">
+        <v>74</v>
       </c>
       <c r="G36">
-        <v>1.71</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H36">
-        <v>1.71</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>72</v>
-      </c>
-      <c r="F37" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G37">
-        <v>2.2999999999999998</v>
+        <v>0.2301</v>
       </c>
       <c r="H37">
-        <v>2.2999999999999998</v>
+        <v>0.2301</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G38">
         <v>0.75839999999999996</v>
@@ -1650,42 +1641,36 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
-      </c>
-      <c r="G39">
-        <v>0.41</v>
-      </c>
-      <c r="H39">
-        <v>0.41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G40">
         <v>0.95330000000000004</v>

</xml_diff>